<commit_message>
Button lock + Door modules I2C communication
</commit_message>
<xml_diff>
--- a/Settings.xlsx
+++ b/Settings.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\larp_secure_doors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D86718E-9856-4ED1-805B-26E719550EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74317C3D-BDEE-48B0-8EC2-A056CDD49F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1344" yWindow="-108" windowWidth="21804" windowHeight="13176" xr2:uid="{EE5008F3-9754-4420-B3C3-2E2BF7827494}"/>
+    <workbookView xWindow="1344" yWindow="-108" windowWidth="21804" windowHeight="13176" activeTab="1" xr2:uid="{EE5008F3-9754-4420-B3C3-2E2BF7827494}"/>
   </bookViews>
   <sheets>
     <sheet name="Door delays" sheetId="1" r:id="rId1"/>
+    <sheet name="Pins" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,9 +36,147 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Евгений Рожков</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{138D25A0-B7C6-42E6-B0B3-F43B037CBC47}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Евгений Рожков:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Beyound MVP</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>Code lock</t>
+  </si>
+  <si>
+    <t>Button lock</t>
+  </si>
+  <si>
+    <t>RFID lock</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Open button</t>
+  </si>
+  <si>
+    <t>Close button</t>
+  </si>
+  <si>
+    <t>I2C SDA</t>
+  </si>
+  <si>
+    <t>I2C SCL</t>
+  </si>
+  <si>
+    <t>Digital keyboard</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>RFID SS</t>
+  </si>
+  <si>
+    <t>RFID RST</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +184,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +238,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D348B51-9F6A-4BE1-BE3A-FC0A3CBF6F17}">
   <dimension ref="A1:E256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2038,4 +2216,267 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3C7458-B055-4B65-ACDE-D7349D1EF8F7}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="5" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>